<commit_message>
update output commodity to h2gc for the trade links
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B809E12D-136B-4F39-BB1C-18E14013E511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9916A0BA-C214-43C0-9D90-33A6ECC8BF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16356" yWindow="1560" windowWidth="21012" windowHeight="14256" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17052" yWindow="2256" windowWidth="21012" windowHeight="14256" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -190,28 +190,28 @@
     <t>FIXOM</t>
   </si>
   <si>
-    <t>TB_H2_DKISLBH_DKE_01</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISLBH_DKE_02</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISL1_DKW_01</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISL1_DKW_02</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISL2_DKW_01</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISL2_DKW_02</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISL3_DKW_01</t>
-  </si>
-  <si>
-    <t>TB_H2_DKISL3_DKW_02</t>
+    <t>TB_H2GC_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_H2GC_DKISL3_DKW_02</t>
   </si>
 </sst>
 </file>
@@ -840,8 +840,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +988,7 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13" t="str">
         <f>O4</f>
-        <v>TB_H2_DKISLBH_DKE_01</v>
+        <v>TB_H2GC_DKISLBH_DKE_01</v>
       </c>
       <c r="P5" s="13"/>
     </row>
@@ -1013,7 +1013,7 @@
       <c r="N6" s="13"/>
       <c r="O6" s="13" t="str">
         <f>O5</f>
-        <v>TB_H2_DKISLBH_DKE_01</v>
+        <v>TB_H2GC_DKISLBH_DKE_01</v>
       </c>
       <c r="P6" s="13"/>
     </row>
@@ -1040,7 +1040,7 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13" t="str">
         <f>O6</f>
-        <v>TB_H2_DKISLBH_DKE_01</v>
+        <v>TB_H2GC_DKISLBH_DKE_01</v>
       </c>
       <c r="P7" s="13"/>
     </row>
@@ -1065,7 +1065,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="14" t="str">
         <f>O7</f>
-        <v>TB_H2_DKISLBH_DKE_01</v>
+        <v>TB_H2GC_DKISLBH_DKE_01</v>
       </c>
       <c r="P8" s="14"/>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="O10" t="str">
         <f>O9</f>
-        <v>TB_H2_DKISLBH_DKE_02</v>
+        <v>TB_H2GC_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O13" si="1">O10</f>
-        <v>TB_H2_DKISLBH_DKE_02</v>
+        <v>TB_H2GC_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="1"/>
-        <v>TB_H2_DKISLBH_DKE_02</v>
+        <v>TB_H2GC_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1163,7 +1163,7 @@
       <c r="N13" s="14"/>
       <c r="O13" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>TB_H2_DKISLBH_DKE_02</v>
+        <v>TB_H2GC_DKISLBH_DKE_02</v>
       </c>
       <c r="P13" s="14"/>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13">
-        <f>I14</f>
+        <f t="shared" ref="K14:K23" si="2">I14</f>
         <v>50</v>
       </c>
       <c r="L14" s="13"/>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13">
-        <f>I15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L15" s="13"/>
@@ -1212,7 +1212,7 @@
       <c r="N15" s="13"/>
       <c r="O15" s="17" t="str">
         <f>O14</f>
-        <v>TB_H2_DKISL1_DKW_01</v>
+        <v>TB_H2GC_DKISL1_DKW_01</v>
       </c>
       <c r="P15" s="13"/>
     </row>
@@ -1229,15 +1229,15 @@
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16">
-        <f>I16</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="17" t="str">
-        <f t="shared" ref="O16:O18" si="2">O15</f>
-        <v>TB_H2_DKISL1_DKW_01</v>
+        <f t="shared" ref="O16:O18" si="3">O15</f>
+        <v>TB_H2GC_DKISL1_DKW_01</v>
       </c>
       <c r="P16" s="13"/>
     </row>
@@ -1256,15 +1256,15 @@
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="16">
-        <f>I17</f>
+        <f t="shared" si="2"/>
         <v>0.98</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>TB_H2_DKISL1_DKW_01</v>
+        <f t="shared" si="3"/>
+        <v>TB_H2GC_DKISL1_DKW_01</v>
       </c>
       <c r="P17" s="13"/>
     </row>
@@ -1281,15 +1281,15 @@
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="14">
-        <f>I18</f>
+        <f t="shared" si="2"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>TB_H2_DKISL1_DKW_01</v>
+        <f t="shared" si="3"/>
+        <v>TB_H2GC_DKISL1_DKW_01</v>
       </c>
       <c r="P18" s="14"/>
     </row>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13">
-        <f>I19</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="L19" s="15"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13">
-        <f>I20</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L20" s="13"/>
@@ -1338,7 +1338,7 @@
       <c r="N20" s="13"/>
       <c r="O20" s="17" t="str">
         <f>O19</f>
-        <v>TB_H2_DKISL1_DKW_02</v>
+        <v>TB_H2GC_DKISL1_DKW_02</v>
       </c>
       <c r="P20" s="13"/>
     </row>
@@ -1355,15 +1355,15 @@
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="18">
-        <f>I21</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L21" s="16"/>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
       <c r="O21" s="17" t="str">
-        <f t="shared" ref="O21:O23" si="3">O20</f>
-        <v>TB_H2_DKISL1_DKW_02</v>
+        <f t="shared" ref="O21:O23" si="4">O20</f>
+        <v>TB_H2GC_DKISL1_DKW_02</v>
       </c>
       <c r="P21" s="13"/>
     </row>
@@ -1382,15 +1382,15 @@
       </c>
       <c r="J22" s="16"/>
       <c r="K22" s="18">
-        <f>I22</f>
+        <f t="shared" si="2"/>
         <v>0.98</v>
       </c>
       <c r="L22" s="16"/>
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
       <c r="O22" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v>TB_H2_DKISL1_DKW_02</v>
+        <f t="shared" si="4"/>
+        <v>TB_H2GC_DKISL1_DKW_02</v>
       </c>
       <c r="P22" s="13"/>
     </row>
@@ -1407,15 +1407,15 @@
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="14">
-        <f>I23</f>
+        <f t="shared" si="2"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
       <c r="O23" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v>TB_H2_DKISL1_DKW_02</v>
+        <f t="shared" si="4"/>
+        <v>TB_H2GC_DKISL1_DKW_02</v>
       </c>
       <c r="P23" s="14"/>
     </row>
@@ -1464,7 +1464,7 @@
       <c r="N25" s="13"/>
       <c r="O25" s="13" t="str">
         <f>O24</f>
-        <v>TB_H2_DKISL2_DKW_01</v>
+        <v>TB_H2GC_DKISL2_DKW_01</v>
       </c>
       <c r="P25" s="13"/>
     </row>
@@ -1482,14 +1482,14 @@
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="13">
-        <f t="shared" ref="L26:L28" si="4">I26</f>
+        <f t="shared" ref="L26:L28" si="5">I26</f>
         <v>0</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13" t="str">
-        <f t="shared" ref="O26:O28" si="5">O25</f>
-        <v>TB_H2_DKISL2_DKW_01</v>
+        <f t="shared" ref="O26:O28" si="6">O25</f>
+        <v>TB_H2GC_DKISL2_DKW_01</v>
       </c>
       <c r="P26" s="13"/>
     </row>
@@ -1509,14 +1509,14 @@
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.98</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>TB_H2_DKISL2_DKW_01</v>
+        <f t="shared" si="6"/>
+        <v>TB_H2GC_DKISL2_DKW_01</v>
       </c>
       <c r="P27" s="13"/>
     </row>
@@ -1534,14 +1534,14 @@
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
       <c r="O28" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>TB_H2_DKISL2_DKW_01</v>
+        <f t="shared" si="6"/>
+        <v>TB_H2GC_DKISL2_DKW_01</v>
       </c>
       <c r="P28" s="14"/>
     </row>
@@ -1590,7 +1590,7 @@
       <c r="N30" s="13"/>
       <c r="O30" s="13" t="str">
         <f>O29</f>
-        <v>TB_H2_DKISL2_DKW_02</v>
+        <v>TB_H2GC_DKISL2_DKW_02</v>
       </c>
       <c r="P30" s="13"/>
     </row>
@@ -1608,14 +1608,14 @@
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="17">
-        <f t="shared" ref="L31:L33" si="6">I31</f>
+        <f t="shared" ref="L31:L33" si="7">I31</f>
         <v>1</v>
       </c>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13" t="str">
-        <f t="shared" ref="O31:O33" si="7">O30</f>
-        <v>TB_H2_DKISL2_DKW_02</v>
+        <f t="shared" ref="O31:O33" si="8">O30</f>
+        <v>TB_H2GC_DKISL2_DKW_02</v>
       </c>
       <c r="P31" s="13"/>
     </row>
@@ -1635,14 +1635,14 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.98</v>
       </c>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13" t="str">
-        <f t="shared" si="7"/>
-        <v>TB_H2_DKISL2_DKW_02</v>
+        <f t="shared" si="8"/>
+        <v>TB_H2GC_DKISL2_DKW_02</v>
       </c>
       <c r="P32" s="13"/>
     </row>
@@ -1660,14 +1660,14 @@
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
       <c r="L33" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M33" s="14"/>
       <c r="N33" s="14"/>
       <c r="O33" s="13" t="str">
-        <f t="shared" si="7"/>
-        <v>TB_H2_DKISL2_DKW_02</v>
+        <f t="shared" si="8"/>
+        <v>TB_H2GC_DKISL2_DKW_02</v>
       </c>
       <c r="P33" s="14"/>
     </row>
@@ -1716,7 +1716,7 @@
       <c r="N35" s="13"/>
       <c r="O35" s="13" t="str">
         <f>O34</f>
-        <v>TB_H2_DKISL3_DKW_01</v>
+        <v>TB_H2GC_DKISL3_DKW_01</v>
       </c>
       <c r="P35" s="13"/>
     </row>
@@ -1735,13 +1735,13 @@
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13">
-        <f t="shared" ref="M36:M38" si="8">I36</f>
+        <f t="shared" ref="M36:M38" si="9">I36</f>
         <v>0</v>
       </c>
       <c r="N36" s="13"/>
       <c r="O36" s="13" t="str">
-        <f t="shared" ref="O36:O38" si="9">O35</f>
-        <v>TB_H2_DKISL3_DKW_01</v>
+        <f t="shared" ref="O36:O38" si="10">O35</f>
+        <v>TB_H2GC_DKISL3_DKW_01</v>
       </c>
       <c r="P36" s="13"/>
     </row>
@@ -1762,13 +1762,13 @@
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.98</v>
       </c>
       <c r="N37" s="13"/>
       <c r="O37" s="13" t="str">
-        <f t="shared" si="9"/>
-        <v>TB_H2_DKISL3_DKW_01</v>
+        <f t="shared" si="10"/>
+        <v>TB_H2GC_DKISL3_DKW_01</v>
       </c>
       <c r="P37" s="13"/>
     </row>
@@ -1787,13 +1787,13 @@
       <c r="K38" s="14"/>
       <c r="L38" s="14"/>
       <c r="M38" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="N38" s="14"/>
       <c r="O38" s="13" t="str">
-        <f t="shared" si="9"/>
-        <v>TB_H2_DKISL3_DKW_01</v>
+        <f t="shared" si="10"/>
+        <v>TB_H2GC_DKISL3_DKW_01</v>
       </c>
       <c r="P38" s="14"/>
     </row>
@@ -1842,7 +1842,7 @@
       <c r="N40" s="13"/>
       <c r="O40" s="13" t="str">
         <f>O39</f>
-        <v>TB_H2_DKISL3_DKW_02</v>
+        <v>TB_H2GC_DKISL3_DKW_02</v>
       </c>
       <c r="P40" s="13"/>
     </row>
@@ -1861,13 +1861,13 @@
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
       <c r="M41" s="17">
-        <f t="shared" ref="M41:M43" si="10">I41</f>
+        <f t="shared" ref="M41:M43" si="11">I41</f>
         <v>1</v>
       </c>
       <c r="N41" s="13"/>
       <c r="O41" s="13" t="str">
-        <f t="shared" ref="O41:O43" si="11">O40</f>
-        <v>TB_H2_DKISL3_DKW_02</v>
+        <f t="shared" ref="O41:O43" si="12">O40</f>
+        <v>TB_H2GC_DKISL3_DKW_02</v>
       </c>
       <c r="P41" s="13"/>
     </row>
@@ -1888,13 +1888,13 @@
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
       <c r="M42" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.98</v>
       </c>
       <c r="N42" s="13"/>
       <c r="O42" s="13" t="str">
-        <f t="shared" si="11"/>
-        <v>TB_H2_DKISL3_DKW_02</v>
+        <f t="shared" si="12"/>
+        <v>TB_H2GC_DKISL3_DKW_02</v>
       </c>
       <c r="P42" s="13"/>
     </row>
@@ -1913,13 +1913,13 @@
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
       <c r="M43" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="N43" s="14"/>
-      <c r="O43" s="13" t="str">
-        <f t="shared" si="11"/>
-        <v>TB_H2_DKISL3_DKW_02</v>
+      <c r="O43" s="14" t="str">
+        <f t="shared" si="12"/>
+        <v>TB_H2GC_DKISL3_DKW_02</v>
       </c>
       <c r="P43" s="14"/>
     </row>

</xml_diff>

<commit_message>
Update prices for pipe & Ship Transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C8939F-EA8D-4E74-9689-97EF2E304CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19562213-9A1B-40EE-88E3-A8DE8FB8FFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17052" yWindow="2256" windowWidth="21012" windowHeight="14256" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,6 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -841,7 +842,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,12 +976,12 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13">
-        <v>0</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13">
         <f>H5</f>
-        <v>0</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -1000,12 +1001,12 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13">
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13">
         <f t="shared" ref="J6:J8" si="0">H6</f>
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -1075,12 +1076,12 @@
       </c>
       <c r="E9" s="11"/>
       <c r="H9" s="11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11">
         <f>H9</f>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O9" t="s">
         <v>36</v>
@@ -1092,12 +1093,12 @@
       </c>
       <c r="E10" s="13"/>
       <c r="H10" s="17">
-        <v>1</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13">
         <f>H10</f>
-        <v>1</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="O10" t="str">
         <f>O9</f>
@@ -1109,13 +1110,13 @@
         <v>34</v>
       </c>
       <c r="E11" s="13"/>
-      <c r="H11" s="17">
-        <v>1</v>
+      <c r="H11" s="20">
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="17">
         <f>H11</f>
-        <v>1</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O13" si="1">O10</f>
@@ -1200,12 +1201,12 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
-        <v>0</v>
+        <v>0.29830000000000001</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.29830000000000001</v>
       </c>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
@@ -1225,12 +1226,12 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13">
-        <v>0</v>
+        <v>1.9000000000000001E-4</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.9000000000000001E-4</v>
       </c>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
@@ -1302,12 +1303,12 @@
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
@@ -1326,12 +1327,13 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="17">
-        <v>1</v>
+        <f>H10</f>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1350,13 +1352,14 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="17">
-        <v>1</v>
+      <c r="I21" s="20">
+        <f>H11</f>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="L21" s="16"/>
       <c r="M21" s="13"/>
@@ -1452,13 +1455,13 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="17">
-        <v>0</v>
+        <v>0.38779999999999998</v>
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13">
         <f>I25</f>
-        <v>0</v>
+        <v>0.38779999999999998</v>
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
@@ -1477,13 +1480,13 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="17">
-        <v>0</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="13">
         <f t="shared" ref="L26:L28" si="5">I26</f>
-        <v>0</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="13"/>
@@ -1554,13 +1557,13 @@
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15">
         <f>I29</f>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
@@ -1578,13 +1581,14 @@
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="17">
-        <v>1</v>
+        <f>I20</f>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="17">
         <f>I30</f>
-        <v>1</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
@@ -1602,14 +1606,15 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="17">
-        <v>1</v>
+      <c r="I31" s="20">
+        <f>I21</f>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="17">
         <f t="shared" ref="L31:L33" si="7">I31</f>
-        <v>1</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
@@ -1704,14 +1709,14 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="17">
-        <v>0</v>
+        <v>5370</v>
       </c>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13">
         <f>I35</f>
-        <v>0</v>
+        <v>5370</v>
       </c>
       <c r="N35" s="13"/>
       <c r="O35" s="13" t="str">
@@ -1729,14 +1734,14 @@
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="17">
-        <v>0</v>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13">
         <f t="shared" ref="M36:M38" si="9">I36</f>
-        <v>0</v>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="N36" s="13"/>
       <c r="O36" s="13" t="str">
@@ -1806,14 +1811,14 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15">
         <f>I39</f>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="N39" s="15"/>
       <c r="O39" s="15" t="s">
@@ -1830,14 +1835,15 @@
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="17">
-        <v>1</v>
+        <f>I20</f>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
       <c r="M40" s="17">
         <f>I40</f>
-        <v>1</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="N40" s="13"/>
       <c r="O40" s="13" t="str">
@@ -1854,15 +1860,16 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="17">
-        <v>1</v>
+      <c r="I41" s="20">
+        <f>I21</f>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
       <c r="M41" s="17">
         <f t="shared" ref="M41:M43" si="11">I41</f>
-        <v>1</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="N41" s="13"/>
       <c r="O41" s="13" t="str">

</xml_diff>

<commit_message>
Defining efficiency, lifetime etc for the ammonia, methanol, jetfuel tradelinks
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F86A42A-4780-4F06-A420-3F67D89A9626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A61F31-3C86-439F-954A-29E6A870E01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="4980" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
-    <sheet name="SUP_TRADE" sheetId="2" r:id="rId2"/>
+    <sheet name="H2_SUP_TRADE" sheetId="2" r:id="rId2"/>
+    <sheet name="MOE_SUP_TRADE" sheetId="4" r:id="rId3"/>
+    <sheet name="KRE_SUP_TRADE" sheetId="5" r:id="rId4"/>
+    <sheet name="AMM_SUP_TRADE" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,8 +85,161 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Maurizio Gargiulo</author>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{A65FB339-D536-49EC-B012-0600B4DCE5E8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert Table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{95038686-4EFC-4858-9B24-2C4A11E7154E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{A330ACB6-15B1-40AA-8710-9FE882C182E2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Maurizio Gargiulo</author>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{D8C32D1F-FB84-4DB2-BCD9-A9C3C721C3CF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert Table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{5AFEE202-8554-449F-8841-7C070948BD42}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{0BAD7CD0-790A-4B43-883E-422B1830E10A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Maurizio Gargiulo</author>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{53509C0A-C4B9-4343-B8E1-BBC4B1A98694}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert Table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{31D0F415-03EA-4258-8666-C01FB5C35AE0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{02FCD11E-A241-443F-AAAA-C04304FF1858}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="67">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -212,6 +368,78 @@
   </si>
   <si>
     <t>TB_H2_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_MOE_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_KRE_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_AMM_DKISL3_DKW_02</t>
   </si>
 </sst>
 </file>
@@ -823,7 +1051,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>ADDRESS(ROW(SUP_TRADE!H3),COLUMN(SUP_TRADE!H3),4,1)&amp;","&amp;ADDRESS(ROW(SUP_TRADE!I3),COLUMN(SUP_TRADE!I3),4,1)</f>
+        <f>ADDRESS(ROW(H2_SUP_TRADE!H3),COLUMN(H2_SUP_TRADE!H3),4,1)&amp;","&amp;ADDRESS(ROW(H2_SUP_TRADE!I3),COLUMN(H2_SUP_TRADE!I3),4,1)</f>
         <v>H3,I3</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -839,10 +1067,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V43"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,12 +1092,12 @@
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -882,7 +1110,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -944,7 +1172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
@@ -968,7 +1196,7 @@
       <c r="P4" s="11"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>33</v>
       </c>
@@ -993,7 +1221,7 @@
       </c>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D6" s="12" t="s">
         <v>34</v>
       </c>
@@ -1018,7 +1246,7 @@
       </c>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
@@ -1045,7 +1273,7 @@
       </c>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="14" t="s">
         <v>17</v>
       </c>
@@ -1070,7 +1298,7 @@
       </c>
       <c r="P8" s="14"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
@@ -1087,7 +1315,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
         <v>33</v>
       </c>
@@ -1104,11 +1332,8 @@
         <f>O9</f>
         <v>TB_H2_DKISLBH_DKE_02</v>
       </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" s="12" t="s">
         <v>34</v>
       </c>
@@ -1126,7 +1351,7 @@
         <v>TB_H2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
@@ -1146,7 +1371,7 @@
         <v>TB_H2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="14" t="s">
         <v>17</v>
       </c>
@@ -1171,7 +1396,7 @@
       </c>
       <c r="P13" s="14"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" s="11" t="s">
         <v>18</v>
       </c>
@@ -1195,7 +1420,7 @@
       </c>
       <c r="P14" s="13"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D15" s="12" t="s">
         <v>33</v>
       </c>
@@ -1220,7 +1445,7 @@
       </c>
       <c r="P15" s="13"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D16" s="12" t="s">
         <v>34</v>
       </c>
@@ -1938,4 +2163,2908 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631640E5-5850-40C9-881C-CA46D9462D7F}">
+  <dimension ref="C2:V43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:O43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="I4" s="11">
+        <v>50</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11">
+        <v>50</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="I5" s="13">
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13">
+        <f>I5</f>
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" t="str">
+        <f>P4</f>
+        <v>TB_MOE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="I6" s="13">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6:K8" si="0">I6</f>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P8" si="1">P5</f>
+        <v>TB_MOE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_MOE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="I8" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_MOE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="I9" s="11">
+        <v>20</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11">
+        <f>I9</f>
+        <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="I10" s="17">
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13">
+        <f>I10</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="P10" t="str">
+        <f>P9</f>
+        <v>TB_MOE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="I11" s="20">
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="17">
+        <f>I11</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ref="P11:P13" si="2">P10</f>
+        <v>TB_MOE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
+        <f>I12</f>
+        <v>0.98</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_MOE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="I13" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14">
+        <f>I13</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_MOE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="11">
+        <v>50</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13">
+        <f t="shared" ref="L14:L23" si="3">J14</f>
+        <v>50</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13">
+        <f t="shared" si="3"/>
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" t="str">
+        <f>P14</f>
+        <v>TB_MOE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16">
+        <f t="shared" si="3"/>
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" t="str">
+        <f t="shared" ref="P16:P18" si="4">P15</f>
+        <v>TB_MOE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_MOE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="18" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_MOE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="11">
+        <v>20</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="17">
+        <f>I10</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13">
+        <f t="shared" si="3"/>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" t="str">
+        <f>P19</f>
+        <v>TB_MOE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="20">
+        <f>I11</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K21" s="16"/>
+      <c r="L21" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21:P23" si="5">P20</f>
+        <v>TB_MOE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="18">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="M22" s="16"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_MOE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="23" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_MOE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="11">
+        <v>50</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15">
+        <f>J24</f>
+        <v>50</v>
+      </c>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="17">
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13">
+        <f>J25</f>
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" t="str">
+        <f>P24</f>
+        <v>TB_MOE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="17">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="13">
+        <f t="shared" ref="M26:M28" si="6">J26</f>
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N26" s="16"/>
+      <c r="O26" s="13"/>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26:P28" si="7">P25</f>
+        <v>TB_MOE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="13">
+        <f t="shared" si="6"/>
+        <v>0.98</v>
+      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="13"/>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_MOE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="28" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="13">
+        <f t="shared" si="6"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_MOE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="11">
+        <v>20</v>
+      </c>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15">
+        <f>J29</f>
+        <v>20</v>
+      </c>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="17">
+        <f>J20</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="17">
+        <f>J30</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" t="str">
+        <f>P29</f>
+        <v>TB_MOE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="31" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="20">
+        <f>J21</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="17">
+        <f t="shared" ref="M31:M33" si="8">J31</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" t="str">
+        <f t="shared" ref="P31:P33" si="9">P30</f>
+        <v>TB_MOE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="32" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="17">
+        <f t="shared" si="8"/>
+        <v>0.98</v>
+      </c>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" t="str">
+        <f t="shared" si="9"/>
+        <v>TB_MOE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="17">
+        <f t="shared" si="8"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" t="str">
+        <f t="shared" si="9"/>
+        <v>TB_MOE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="11">
+        <v>50</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15">
+        <f>J34</f>
+        <v>50</v>
+      </c>
+      <c r="O34" s="15"/>
+      <c r="P34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="17">
+        <v>5370</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13">
+        <f>J35</f>
+        <v>5370</v>
+      </c>
+      <c r="O35" s="13"/>
+      <c r="P35" t="str">
+        <f>P34</f>
+        <v>TB_MOE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="17">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13">
+        <f t="shared" ref="N36:N38" si="10">J36</f>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="O36" s="13"/>
+      <c r="P36" t="str">
+        <f t="shared" ref="P36:P38" si="11">P35</f>
+        <v>TB_MOE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13">
+        <f t="shared" si="10"/>
+        <v>0.98</v>
+      </c>
+      <c r="O37" s="13"/>
+      <c r="P37" t="str">
+        <f t="shared" si="11"/>
+        <v>TB_MOE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="13">
+        <f t="shared" si="10"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O38" s="14"/>
+      <c r="P38" t="str">
+        <f t="shared" si="11"/>
+        <v>TB_MOE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="11">
+        <v>20</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15">
+        <f>J39</f>
+        <v>20</v>
+      </c>
+      <c r="O39" s="15"/>
+      <c r="P39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E40" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="17">
+        <f>J20</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="17">
+        <f>J40</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="O40" s="13"/>
+      <c r="P40" t="str">
+        <f>P39</f>
+        <v>TB_MOE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E41" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="20">
+        <f>J21</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="17">
+        <f t="shared" ref="N41:N43" si="12">J41</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="O41" s="13"/>
+      <c r="P41" t="str">
+        <f t="shared" ref="P41:P43" si="13">P40</f>
+        <v>TB_MOE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="17">
+        <f t="shared" si="12"/>
+        <v>0.98</v>
+      </c>
+      <c r="O42" s="13"/>
+      <c r="P42" t="str">
+        <f t="shared" si="13"/>
+        <v>TB_MOE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E43" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="19">
+        <f t="shared" si="12"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O43" s="14"/>
+      <c r="P43" t="str">
+        <f t="shared" si="13"/>
+        <v>TB_MOE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6708D45-E573-4DB0-9E7B-7DC3BD947BD4}">
+  <dimension ref="C2:V43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:O43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="I4" s="11">
+        <v>50</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11">
+        <v>50</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="I5" s="13">
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13">
+        <f>I5</f>
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" t="str">
+        <f>P4</f>
+        <v>TB_KRE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="I6" s="13">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6:K8" si="0">I6</f>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P8" si="1">P5</f>
+        <v>TB_KRE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_KRE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="I8" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_KRE_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="I9" s="11">
+        <v>20</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11">
+        <f>I9</f>
+        <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="I10" s="17">
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13">
+        <f>I10</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="P10" t="str">
+        <f>P9</f>
+        <v>TB_KRE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="I11" s="20">
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="17">
+        <f>I11</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ref="P11:P13" si="2">P10</f>
+        <v>TB_KRE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
+        <f>I12</f>
+        <v>0.98</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_KRE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="I13" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14">
+        <f>I13</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_KRE_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="11">
+        <v>50</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13">
+        <f t="shared" ref="L14:L23" si="3">J14</f>
+        <v>50</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13">
+        <f t="shared" si="3"/>
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" t="str">
+        <f>P14</f>
+        <v>TB_KRE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16">
+        <f t="shared" si="3"/>
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" t="str">
+        <f t="shared" ref="P16:P18" si="4">P15</f>
+        <v>TB_KRE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_KRE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="18" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_KRE_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="11">
+        <v>20</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="17">
+        <f>I10</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13">
+        <f t="shared" si="3"/>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" t="str">
+        <f>P19</f>
+        <v>TB_KRE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="20">
+        <f>I11</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K21" s="16"/>
+      <c r="L21" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21:P23" si="5">P20</f>
+        <v>TB_KRE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="18">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="M22" s="16"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_KRE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="23" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_KRE_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="11">
+        <v>50</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15">
+        <f>J24</f>
+        <v>50</v>
+      </c>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="17">
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13">
+        <f>J25</f>
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" t="str">
+        <f>P24</f>
+        <v>TB_KRE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="17">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="13">
+        <f t="shared" ref="M26:M28" si="6">J26</f>
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N26" s="16"/>
+      <c r="O26" s="13"/>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26:P28" si="7">P25</f>
+        <v>TB_KRE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="13">
+        <f t="shared" si="6"/>
+        <v>0.98</v>
+      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="13"/>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_KRE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="28" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="13">
+        <f t="shared" si="6"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_KRE_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="11">
+        <v>20</v>
+      </c>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15">
+        <f>J29</f>
+        <v>20</v>
+      </c>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="17">
+        <f>J20</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="17">
+        <f>J30</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" t="str">
+        <f>P29</f>
+        <v>TB_KRE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="31" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="20">
+        <f>J21</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="17">
+        <f t="shared" ref="M31:M33" si="8">J31</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" t="str">
+        <f t="shared" ref="P31:P33" si="9">P30</f>
+        <v>TB_KRE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="32" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="17">
+        <f t="shared" si="8"/>
+        <v>0.98</v>
+      </c>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" t="str">
+        <f t="shared" si="9"/>
+        <v>TB_KRE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="17">
+        <f t="shared" si="8"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" t="str">
+        <f t="shared" si="9"/>
+        <v>TB_KRE_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="11">
+        <v>50</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15">
+        <f>J34</f>
+        <v>50</v>
+      </c>
+      <c r="O34" s="15"/>
+      <c r="P34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="17">
+        <v>5370</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13">
+        <f>J35</f>
+        <v>5370</v>
+      </c>
+      <c r="O35" s="13"/>
+      <c r="P35" t="str">
+        <f>P34</f>
+        <v>TB_KRE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="17">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13">
+        <f t="shared" ref="N36:N38" si="10">J36</f>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="O36" s="13"/>
+      <c r="P36" t="str">
+        <f t="shared" ref="P36:P38" si="11">P35</f>
+        <v>TB_KRE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13">
+        <f t="shared" si="10"/>
+        <v>0.98</v>
+      </c>
+      <c r="O37" s="13"/>
+      <c r="P37" t="str">
+        <f t="shared" si="11"/>
+        <v>TB_KRE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="13">
+        <f t="shared" si="10"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O38" s="14"/>
+      <c r="P38" t="str">
+        <f t="shared" si="11"/>
+        <v>TB_KRE_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="11">
+        <v>20</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15">
+        <f>J39</f>
+        <v>20</v>
+      </c>
+      <c r="O39" s="15"/>
+      <c r="P39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E40" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="17">
+        <f>J20</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="17">
+        <f>J40</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="O40" s="13"/>
+      <c r="P40" t="str">
+        <f>P39</f>
+        <v>TB_KRE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E41" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="20">
+        <f>J21</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="17">
+        <f t="shared" ref="N41:N43" si="12">J41</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="O41" s="13"/>
+      <c r="P41" t="str">
+        <f t="shared" ref="P41:P43" si="13">P40</f>
+        <v>TB_KRE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="17">
+        <f t="shared" si="12"/>
+        <v>0.98</v>
+      </c>
+      <c r="O42" s="13"/>
+      <c r="P42" t="str">
+        <f t="shared" si="13"/>
+        <v>TB_KRE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E43" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="19">
+        <f t="shared" si="12"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O43" s="14"/>
+      <c r="P43" t="str">
+        <f t="shared" si="13"/>
+        <v>TB_KRE_DKISL3_DKW_02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD4FCC-23F0-4F3B-9CD2-8D3544B74DA5}">
+  <dimension ref="C2:V43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC45" sqref="AC45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="I4" s="11">
+        <v>50</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11">
+        <v>50</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="I5" s="13">
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13">
+        <f>I5</f>
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" t="str">
+        <f>P4</f>
+        <v>TB_AMM_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="I6" s="13">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6:K8" si="0">I6</f>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P8" si="1">P5</f>
+        <v>TB_AMM_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_AMM_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="I8" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_AMM_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="I9" s="11">
+        <v>20</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11">
+        <f>I9</f>
+        <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="I10" s="17">
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13">
+        <f>I10</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="P10" t="str">
+        <f>P9</f>
+        <v>TB_AMM_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="I11" s="20">
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="17">
+        <f>I11</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ref="P11:P13" si="2">P10</f>
+        <v>TB_AMM_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
+        <f>I12</f>
+        <v>0.98</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_AMM_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="I13" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14">
+        <f>I13</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_AMM_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="11">
+        <v>50</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13">
+        <f t="shared" ref="L14:L23" si="3">J14</f>
+        <v>50</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13">
+        <f t="shared" si="3"/>
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" t="str">
+        <f>P14</f>
+        <v>TB_AMM_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16">
+        <f t="shared" si="3"/>
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" t="str">
+        <f t="shared" ref="P16:P18" si="4">P15</f>
+        <v>TB_AMM_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_AMM_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="18" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_AMM_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="11">
+        <v>20</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="17">
+        <f>I10</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13">
+        <f t="shared" si="3"/>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" t="str">
+        <f>P19</f>
+        <v>TB_AMM_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="20">
+        <f>I11</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K21" s="16"/>
+      <c r="L21" s="18">
+        <f t="shared" si="3"/>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21:P23" si="5">P20</f>
+        <v>TB_AMM_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="18">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="M22" s="16"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_AMM_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="23" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_AMM_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="11">
+        <v>50</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15">
+        <f>J24</f>
+        <v>50</v>
+      </c>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="17">
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13">
+        <f>J25</f>
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" t="str">
+        <f>P24</f>
+        <v>TB_AMM_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="17">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="13">
+        <f t="shared" ref="M26:M28" si="6">J26</f>
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N26" s="16"/>
+      <c r="O26" s="13"/>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26:P28" si="7">P25</f>
+        <v>TB_AMM_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="13">
+        <f t="shared" si="6"/>
+        <v>0.98</v>
+      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="13"/>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_AMM_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="28" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="13">
+        <f t="shared" si="6"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_AMM_DKISL2_DKW_01</v>
+      </c>
+    </row>
+    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="11">
+        <v>20</v>
+      </c>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15">
+        <f>J29</f>
+        <v>20</v>
+      </c>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="17">
+        <f>J20</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="17">
+        <f>J30</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" t="str">
+        <f>P29</f>
+        <v>TB_AMM_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="31" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="20">
+        <f>J21</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="17">
+        <f t="shared" ref="M31:M33" si="8">J31</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" t="str">
+        <f t="shared" ref="P31:P33" si="9">P30</f>
+        <v>TB_AMM_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="32" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="17">
+        <f t="shared" si="8"/>
+        <v>0.98</v>
+      </c>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" t="str">
+        <f t="shared" si="9"/>
+        <v>TB_AMM_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="17">
+        <f t="shared" si="8"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" t="str">
+        <f t="shared" si="9"/>
+        <v>TB_AMM_DKISL2_DKW_02</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="11">
+        <v>50</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15">
+        <f>J34</f>
+        <v>50</v>
+      </c>
+      <c r="O34" s="15"/>
+      <c r="P34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="17">
+        <v>5370</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13">
+        <f>J35</f>
+        <v>5370</v>
+      </c>
+      <c r="O35" s="13"/>
+      <c r="P35" t="str">
+        <f>P34</f>
+        <v>TB_AMM_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="17">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13">
+        <f t="shared" ref="N36:N38" si="10">J36</f>
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="O36" s="13"/>
+      <c r="P36" t="str">
+        <f t="shared" ref="P36:P38" si="11">P35</f>
+        <v>TB_AMM_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13">
+        <f t="shared" si="10"/>
+        <v>0.98</v>
+      </c>
+      <c r="O37" s="13"/>
+      <c r="P37" t="str">
+        <f t="shared" si="11"/>
+        <v>TB_AMM_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="13">
+        <f t="shared" si="10"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O38" s="14"/>
+      <c r="P38" t="str">
+        <f t="shared" si="11"/>
+        <v>TB_AMM_DKISL3_DKW_01</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="11">
+        <v>20</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15">
+        <f>J39</f>
+        <v>20</v>
+      </c>
+      <c r="O39" s="15"/>
+      <c r="P39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E40" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="17">
+        <f>J20</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="17">
+        <f>J40</f>
+        <v>3.1329000000000001E-3</v>
+      </c>
+      <c r="O40" s="13"/>
+      <c r="P40" t="str">
+        <f>P39</f>
+        <v>TB_AMM_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E41" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="20">
+        <f>J21</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="17">
+        <f t="shared" ref="N41:N43" si="12">J41</f>
+        <v>1.5659999999999999E-5</v>
+      </c>
+      <c r="O41" s="13"/>
+      <c r="P41" t="str">
+        <f t="shared" ref="P41:P43" si="13">P40</f>
+        <v>TB_AMM_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="17">
+        <f t="shared" si="12"/>
+        <v>0.98</v>
+      </c>
+      <c r="O42" s="13"/>
+      <c r="P42" t="str">
+        <f t="shared" si="13"/>
+        <v>TB_AMM_DKISL3_DKW_02</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E43" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="19">
+        <f t="shared" si="12"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O43" s="14"/>
+      <c r="P43" t="str">
+        <f t="shared" si="13"/>
+        <v>TB_AMM_DKISL3_DKW_02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
include Co2 transport to the islands
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC743C71-D65F-426C-9927-4FB86B3B8D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC16361F-88ED-4A7C-AE47-B553CB50EA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="2616" windowWidth="30960" windowHeight="12204" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="MOE_SUP_TRADE" sheetId="4" r:id="rId3"/>
     <sheet name="KRE_SUP_TRADE" sheetId="5" r:id="rId4"/>
     <sheet name="AMM_SUP_TRADE" sheetId="6" r:id="rId5"/>
+    <sheet name="CO2_SUP_TRADE" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -238,8 +239,59 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Maurizio Gargiulo</author>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{8BE622A1-C090-4F02-BE06-BCDD3D8278B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insert Table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="1" shapeId="0" xr:uid="{14372D9E-7196-4673-829F-3ABF3F999546}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="1" shapeId="0" xr:uid="{999894EA-5A29-4C06-B887-DEDD13E51398}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="76">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -443,6 +495,30 @@
   </si>
   <si>
     <t>VAROM</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_CO2_DKISL3_DKW_02</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1153,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:N43"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2312,7 +2388,7 @@
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13">
-        <f t="shared" ref="K6:K8" si="0">I6</f>
+        <f t="shared" ref="K6" si="0">I6</f>
         <v>0</v>
       </c>
       <c r="L6" s="13"/>
@@ -2320,7 +2396,7 @@
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" t="str">
-        <f t="shared" ref="P6:P8" si="1">P5</f>
+        <f t="shared" ref="P6:P7" si="1">P5</f>
         <v>TB_MOE_DKISLBH_DKE_01</v>
       </c>
       <c r="AD6" t="str">
@@ -3357,8 +3433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6708D45-E573-4DB0-9E7B-7DC3BD947BD4}">
   <dimension ref="C2:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3493,7 +3569,7 @@
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13">
-        <f t="shared" ref="K6:K8" si="0">I6</f>
+        <f t="shared" ref="K6:K7" si="0">I6</f>
         <v>0</v>
       </c>
       <c r="L6" s="13"/>
@@ -3501,7 +3577,7 @@
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" t="str">
-        <f t="shared" ref="P6:P8" si="1">P5</f>
+        <f t="shared" ref="P6:P7" si="1">P5</f>
         <v>TB_KRE_DKISLBH_DKE_01</v>
       </c>
       <c r="AB6" t="str">
@@ -4448,7 +4524,7 @@
   <dimension ref="C2:AA44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4583,7 +4659,7 @@
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13">
-        <f t="shared" ref="K6:K8" si="0">I6</f>
+        <f t="shared" ref="K6" si="0">I6</f>
         <v>0</v>
       </c>
       <c r="L6" s="13"/>
@@ -4591,7 +4667,7 @@
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" t="str">
-        <f t="shared" ref="P6:P8" si="1">P5</f>
+        <f t="shared" ref="P6:P7" si="1">P5</f>
         <v>TB_AMM_DKISLBH_DKE_01</v>
       </c>
       <c r="AA6" t="str">
@@ -5537,4 +5613,832 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AE1A95-6D3E-474D-AE6A-92E967540746}">
+  <dimension ref="B2:U51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="J4">
+        <f>H4</f>
+        <v>40</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J15" si="0">H5</f>
+        <v>0</v>
+      </c>
+      <c r="O5" t="str">
+        <f>O4</f>
+        <v>TB_CO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" ref="O6:O9" si="1">O5</f>
+        <v>TB_CO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_CO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2020</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_CO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="H9" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_CO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" t="str">
+        <f>O10</f>
+        <v>TB_CO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" ref="O12:O15" si="2">O11</f>
+        <v>TB_CO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_CO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="13">
+        <v>2020</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_CO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="H15" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_CO2_DKISLBH_DKE_02</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="I16">
+        <v>40</v>
+      </c>
+      <c r="K16">
+        <f>I16</f>
+        <v>40</v>
+      </c>
+      <c r="O16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17:K27" si="3">I17</f>
+        <v>0</v>
+      </c>
+      <c r="O17" t="str">
+        <f>O16</f>
+        <v>TB_CO2_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" ref="O18:O21" si="4">O17</f>
+        <v>TB_CO2_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_CO2_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I20" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_CO2_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="I21" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_CO2_DKISL1_DKW_01</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="I22">
+        <v>40</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="O22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O23" t="str">
+        <f>O22</f>
+        <v>TB_CO2_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" ref="O24:O27" si="5">O23</f>
+        <v>TB_CO2_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_CO2_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I26" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_CO2_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="I27" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_CO2_DKISL1_DKW_02</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="I28">
+        <v>40</v>
+      </c>
+      <c r="L28">
+        <f>I28</f>
+        <v>40</v>
+      </c>
+      <c r="O28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L39" si="6">I29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D30" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I32" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="6"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="I33" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="6"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="I34">
+        <v>40</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="O34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D35" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D36" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I38" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="6"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="I39" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="6"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="I40">
+        <v>40</v>
+      </c>
+      <c r="M40">
+        <f>I40</f>
+        <v>40</v>
+      </c>
+      <c r="O40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D41" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <f t="shared" ref="M41:M51" si="7">I41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D42" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D44" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I44" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="7"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="I45" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="7"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D46" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="I46">
+        <v>40</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="O46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D47" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D48" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D50" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="13">
+        <v>2020</v>
+      </c>
+      <c r="I50" s="13">
+        <v>0.98</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="7"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D51" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="I51" s="13">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="7"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change pipe h2 transport price for island 2 and 3
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC16361F-88ED-4A7C-AE47-B553CB50EA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC0D019-133C-4530-AB4E-8A03B6CF4792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="2616" windowWidth="30960" windowHeight="12204" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8628" yWindow="3696" windowWidth="30960" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -525,8 +525,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -706,7 +708,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -740,6 +742,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1152,8 +1156,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1540,7 +1544,7 @@
         <v>1.9000000000000001E-4</v>
       </c>
       <c r="J16" s="16"/>
-      <c r="K16" s="16">
+      <c r="K16" s="25">
         <f t="shared" si="2"/>
         <v>1.9000000000000001E-4</v>
       </c>
@@ -1668,7 +1672,7 @@
         <v>1.5659999999999999E-5</v>
       </c>
       <c r="J21" s="16"/>
-      <c r="K21" s="18">
+      <c r="K21" s="26">
         <f t="shared" si="2"/>
         <v>1.5659999999999999E-5</v>
       </c>
@@ -2020,14 +2024,14 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="17">
-        <v>5370</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13">
         <f>I35</f>
-        <v>5370</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="N35" s="13"/>
       <c r="O35" s="13" t="str">
@@ -2252,7 +2256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631640E5-5850-40C9-881C-CA46D9462D7F}">
   <dimension ref="C2:AD44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
@@ -3433,7 +3437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6708D45-E573-4DB0-9E7B-7DC3BD947BD4}">
   <dimension ref="C2:AB44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -4523,7 +4527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD4FCC-23F0-4F3B-9CD2-8D3544B74DA5}">
   <dimension ref="C2:AA44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
@@ -5619,7 +5623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AE1A95-6D3E-474D-AE6A-92E967540746}">
   <dimension ref="B2:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update co2 process name in SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A35C81-2B4F-4E2E-92CB-834B377FAD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6372E405-7582-4C7C-9599-DDBDCEF5F1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8628" yWindow="3696" windowWidth="30960" windowHeight="12204" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7164" yWindow="2004" windowWidth="30960" windowHeight="12204" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -497,28 +497,28 @@
     <t>VAROM</t>
   </si>
   <si>
-    <t>TB_CO2_DKISLBH_DKE_01</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISLBH_DKE_02</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISL1_DKW_01</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISL1_DKW_02</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISL2_DKW_01</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISL2_DKW_02</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISL3_DKW_01</t>
-  </si>
-  <si>
-    <t>TB_CO2_DKISL3_DKW_02</t>
+    <t>TB_SUPCO2_DKISLBH_DKE_01</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISLBH_DKE_02</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISL1_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISL1_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISL2_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISL2_DKW_02</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISL3_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_SUPCO2_DKISL3_DKW_02</t>
   </si>
 </sst>
 </file>
@@ -5623,8 +5623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AE1A95-6D3E-474D-AE6A-92E967540746}">
   <dimension ref="B2:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S53" sqref="S53"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="O5" t="str">
         <f>O4</f>
-        <v>TB_CO2_DKISLBH_DKE_01</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
@@ -5751,7 +5751,7 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" ref="O6:O9" si="1">O5</f>
-        <v>TB_CO2_DKISLBH_DKE_01</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.3">
@@ -5767,7 +5767,7 @@
       </c>
       <c r="O7" t="str">
         <f t="shared" si="1"/>
-        <v>TB_CO2_DKISLBH_DKE_01</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.3">
@@ -5775,7 +5775,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="H8" s="13">
         <v>0.98</v>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="1"/>
-        <v>TB_CO2_DKISLBH_DKE_01</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" si="1"/>
-        <v>TB_CO2_DKISLBH_DKE_01</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="O11" t="str">
         <f>O10</f>
-        <v>TB_CO2_DKISLBH_DKE_02</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" ref="O12:O15" si="2">O11</f>
-        <v>TB_CO2_DKISLBH_DKE_02</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.3">
@@ -5869,7 +5869,7 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v>TB_CO2_DKISLBH_DKE_02</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
@@ -5877,7 +5877,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="H14" s="13">
         <v>0.98</v>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="2"/>
-        <v>TB_CO2_DKISLBH_DKE_02</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5905,7 +5905,7 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="2"/>
-        <v>TB_CO2_DKISLBH_DKE_02</v>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
@@ -5938,7 +5938,7 @@
       </c>
       <c r="O17" t="str">
         <f>O16</f>
-        <v>TB_CO2_DKISL1_DKW_01</v>
+        <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.3">
@@ -5955,7 +5955,7 @@
       </c>
       <c r="O18" t="str">
         <f t="shared" ref="O18:O21" si="4">O17</f>
-        <v>TB_CO2_DKISL1_DKW_01</v>
+        <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.3">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="O19" t="str">
         <f t="shared" si="4"/>
-        <v>TB_CO2_DKISL1_DKW_01</v>
+        <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.3">
@@ -5979,7 +5979,7 @@
         <v>16</v>
       </c>
       <c r="E20" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I20" s="13">
         <v>0.98</v>
@@ -5990,7 +5990,7 @@
       </c>
       <c r="O20" t="str">
         <f t="shared" si="4"/>
-        <v>TB_CO2_DKISL1_DKW_01</v>
+        <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
     <row r="21" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6007,7 +6007,7 @@
       </c>
       <c r="O21" t="str">
         <f t="shared" si="4"/>
-        <v>TB_CO2_DKISL1_DKW_01</v>
+        <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
     <row r="22" spans="4:15" x14ac:dyDescent="0.3">
@@ -6040,7 +6040,7 @@
       </c>
       <c r="O23" t="str">
         <f>O22</f>
-        <v>TB_CO2_DKISL1_DKW_02</v>
+        <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.3">
@@ -6057,7 +6057,7 @@
       </c>
       <c r="O24" t="str">
         <f t="shared" ref="O24:O27" si="5">O23</f>
-        <v>TB_CO2_DKISL1_DKW_02</v>
+        <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.3">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="O25" t="str">
         <f t="shared" si="5"/>
-        <v>TB_CO2_DKISL1_DKW_02</v>
+        <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.3">
@@ -6081,7 +6081,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I26" s="13">
         <v>0.98</v>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="O26" t="str">
         <f t="shared" si="5"/>
-        <v>TB_CO2_DKISL1_DKW_02</v>
+        <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
     <row r="27" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6109,7 +6109,7 @@
       </c>
       <c r="O27" t="str">
         <f t="shared" si="5"/>
-        <v>TB_CO2_DKISL1_DKW_02</v>
+        <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.3">
@@ -6142,7 +6142,7 @@
       </c>
       <c r="O29" t="str">
         <f>O28</f>
-        <v>TB_CO2_DKISL2_DKW_01</v>
+        <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.3">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O33" si="7">O29</f>
-        <v>TB_CO2_DKISL2_DKW_01</v>
+        <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.3">
@@ -6175,7 +6175,7 @@
       </c>
       <c r="O31" t="str">
         <f t="shared" si="7"/>
-        <v>TB_CO2_DKISL2_DKW_01</v>
+        <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.3">
@@ -6183,7 +6183,7 @@
         <v>16</v>
       </c>
       <c r="E32" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I32" s="13">
         <v>0.98</v>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="O32" t="str">
         <f t="shared" si="7"/>
-        <v>TB_CO2_DKISL2_DKW_01</v>
+        <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
     <row r="33" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="O33" t="str">
         <f t="shared" si="7"/>
-        <v>TB_CO2_DKISL2_DKW_01</v>
+        <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.3">
@@ -6244,7 +6244,7 @@
       </c>
       <c r="O35" t="str">
         <f>O34</f>
-        <v>TB_CO2_DKISL2_DKW_02</v>
+        <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.3">
@@ -6261,7 +6261,7 @@
       </c>
       <c r="O36" t="str">
         <f t="shared" ref="O36:O39" si="8">O35</f>
-        <v>TB_CO2_DKISL2_DKW_02</v>
+        <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.3">
@@ -6277,7 +6277,7 @@
       </c>
       <c r="O37" t="str">
         <f t="shared" si="8"/>
-        <v>TB_CO2_DKISL2_DKW_02</v>
+        <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
     <row r="38" spans="4:15" x14ac:dyDescent="0.3">
@@ -6285,7 +6285,7 @@
         <v>16</v>
       </c>
       <c r="E38" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I38" s="13">
         <v>0.98</v>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="O38" t="str">
         <f t="shared" si="8"/>
-        <v>TB_CO2_DKISL2_DKW_02</v>
+        <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
     <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="O39" t="str">
         <f t="shared" si="8"/>
-        <v>TB_CO2_DKISL2_DKW_02</v>
+        <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.3">
@@ -6346,7 +6346,7 @@
       </c>
       <c r="O41" t="str">
         <f>O40</f>
-        <v>TB_CO2_DKISL3_DKW_01</v>
+        <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
     <row r="42" spans="4:15" x14ac:dyDescent="0.3">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="O42" t="str">
         <f t="shared" ref="O42:O45" si="10">O41</f>
-        <v>TB_CO2_DKISL3_DKW_01</v>
+        <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
     <row r="43" spans="4:15" x14ac:dyDescent="0.3">
@@ -6379,7 +6379,7 @@
       </c>
       <c r="O43" t="str">
         <f t="shared" si="10"/>
-        <v>TB_CO2_DKISL3_DKW_01</v>
+        <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.3">
@@ -6387,7 +6387,7 @@
         <v>16</v>
       </c>
       <c r="E44" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I44" s="13">
         <v>0.98</v>
@@ -6398,7 +6398,7 @@
       </c>
       <c r="O44" t="str">
         <f t="shared" si="10"/>
-        <v>TB_CO2_DKISL3_DKW_01</v>
+        <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
     <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6415,7 +6415,7 @@
       </c>
       <c r="O45" t="str">
         <f t="shared" si="10"/>
-        <v>TB_CO2_DKISL3_DKW_01</v>
+        <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
     <row r="46" spans="4:15" x14ac:dyDescent="0.3">
@@ -6448,7 +6448,7 @@
       </c>
       <c r="O47" t="str">
         <f>O46</f>
-        <v>TB_CO2_DKISL3_DKW_02</v>
+        <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
     <row r="48" spans="4:15" x14ac:dyDescent="0.3">
@@ -6465,7 +6465,7 @@
       </c>
       <c r="O48" t="str">
         <f t="shared" ref="O48:O51" si="11">O47</f>
-        <v>TB_CO2_DKISL3_DKW_02</v>
+        <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.3">
@@ -6481,7 +6481,7 @@
       </c>
       <c r="O49" t="str">
         <f t="shared" si="11"/>
-        <v>TB_CO2_DKISL3_DKW_02</v>
+        <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.3">
@@ -6489,7 +6489,7 @@
         <v>16</v>
       </c>
       <c r="E50" s="13">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I50" s="13">
         <v>0.98</v>
@@ -6500,7 +6500,7 @@
       </c>
       <c r="O50" t="str">
         <f t="shared" si="11"/>
-        <v>TB_CO2_DKISL3_DKW_02</v>
+        <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.3">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="O51" t="str">
         <f t="shared" si="11"/>
-        <v>TB_CO2_DKISL3_DKW_02</v>
+        <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include start date for technologies
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6372E405-7582-4C7C-9599-DDBDCEF5F1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223523C6-17EB-4DB5-AD24-E5A4621D776A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7164" yWindow="2004" windowWidth="30960" windowHeight="12204" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="1" shapeId="0" xr:uid="{14372D9E-7196-4673-829F-3ABF3F999546}">
+    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{14372D9E-7196-4673-829F-3ABF3F999546}">
       <text>
         <r>
           <rPr>
@@ -273,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="1" shapeId="0" xr:uid="{999894EA-5A29-4C06-B887-DEDD13E51398}">
+    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{999894EA-5A29-4C06-B887-DEDD13E51398}">
       <text>
         <r>
           <rPr>
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="77">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>TB_SUPCO2_DKISL3_DKW_02</t>
+  </si>
+  <si>
+    <t>START</t>
   </si>
 </sst>
 </file>
@@ -5621,28 +5624,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AE1A95-6D3E-474D-AE6A-92E967540746}">
-  <dimension ref="B2:U51"/>
+  <dimension ref="B2:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
+      <c r="O2" s="2"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
-    </row>
-    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -5656,866 +5659,1013 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="6" t="s">
-        <v>0</v>
-      </c>
       <c r="R3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="H4">
+      <c r="F4" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I4">
         <v>40</v>
       </c>
-      <c r="J4">
-        <f>H4</f>
+      <c r="K4">
+        <f>I4</f>
         <v>40</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D5" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J15" si="0">H5</f>
-        <v>0</v>
-      </c>
-      <c r="O5" t="str">
-        <f>O4</f>
+      <c r="F5" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K15" si="0">I5</f>
+        <v>0</v>
+      </c>
+      <c r="P5" t="str">
+        <f>P4</f>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D6" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="J6">
+      <c r="F6" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" t="str">
-        <f t="shared" ref="O6:O9" si="1">O5</f>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P9" si="1">P5</f>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>67</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="F7" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="1"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="13">
         <v>2030</v>
       </c>
-      <c r="H8" s="13">
+      <c r="F8" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I8" s="13">
         <v>0.98</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="1"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="13"/>
-      <c r="H9" s="13">
+      <c r="F9" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I9" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O9" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="1"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="11"/>
-      <c r="H10">
+      <c r="F10" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I10">
         <v>40</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D11" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="13"/>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="F11" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O11" t="str">
-        <f>O10</f>
+      <c r="P11" t="str">
+        <f>P10</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D12" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="13"/>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="J12">
+      <c r="F12" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O12" t="str">
-        <f t="shared" ref="O12:O15" si="2">O11</f>
+      <c r="P12" t="str">
+        <f t="shared" ref="P12:P15" si="2">P11</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>67</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="J13">
+      <c r="F13" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="2"/>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="13">
         <v>2030</v>
       </c>
-      <c r="H14" s="13">
+      <c r="F14" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I14" s="13">
         <v>0.98</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
-      <c r="O14" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="2"/>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="H15" s="13">
+      <c r="F15" s="13">
+        <v>2030</v>
+      </c>
+      <c r="I15" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O15" t="str">
+      <c r="P15" t="str">
         <f t="shared" si="2"/>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="I16">
+      <c r="F16" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J16">
         <v>40</v>
       </c>
-      <c r="K16">
-        <f>I16</f>
+      <c r="L16">
+        <f>J16</f>
         <v>40</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D17" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <f t="shared" ref="K17:K27" si="3">I17</f>
-        <v>0</v>
-      </c>
-      <c r="O17" t="str">
-        <f>O16</f>
+      <c r="F17" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17:L27" si="3">J17</f>
+        <v>0</v>
+      </c>
+      <c r="P17" t="str">
+        <f>P16</f>
         <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D18" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="K18">
+      <c r="F18" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O18" t="str">
-        <f t="shared" ref="O18:O21" si="4">O17</f>
+      <c r="P18" t="str">
+        <f t="shared" ref="P18:P21" si="4">P17</f>
         <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>67</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="K19">
+      <c r="F19" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O19" t="str">
+      <c r="P19" t="str">
         <f t="shared" si="4"/>
         <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D20" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="13">
         <v>2030</v>
       </c>
-      <c r="I20" s="13">
+      <c r="F20" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J20" s="13">
         <v>0.98</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <f t="shared" si="3"/>
         <v>0.98</v>
       </c>
-      <c r="O20" t="str">
+      <c r="P20" t="str">
         <f t="shared" si="4"/>
         <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
-    <row r="21" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="13"/>
-      <c r="I21" s="13">
+      <c r="F21" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J21" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <f t="shared" si="3"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O21" t="str">
+      <c r="P21" t="str">
         <f t="shared" si="4"/>
         <v>TB_SUPCO2_DKISL1_DKW_01</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D22" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="11"/>
-      <c r="I22">
+      <c r="F22" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J22">
         <v>40</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D23" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="K23">
+      <c r="F23" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O23" t="str">
-        <f>O22</f>
+      <c r="P23" t="str">
+        <f>P22</f>
         <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D24" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="13"/>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="K24">
+      <c r="F24" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O24" t="str">
-        <f t="shared" ref="O24:O27" si="5">O23</f>
+      <c r="P24" t="str">
+        <f t="shared" ref="P24:P27" si="5">P23</f>
         <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>67</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="K25">
+      <c r="F25" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O25" t="str">
+      <c r="P25" t="str">
         <f t="shared" si="5"/>
         <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D26" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="13">
         <v>2030</v>
       </c>
-      <c r="I26" s="13">
+      <c r="F26" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J26" s="13">
         <v>0.98</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <f t="shared" si="3"/>
         <v>0.98</v>
       </c>
-      <c r="O26" t="str">
+      <c r="P26" t="str">
         <f t="shared" si="5"/>
         <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
-    <row r="27" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D27" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="13"/>
-      <c r="I27" s="13">
+      <c r="F27" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J27" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <f t="shared" si="3"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O27" t="str">
+      <c r="P27" t="str">
         <f t="shared" si="5"/>
         <v>TB_SUPCO2_DKISL1_DKW_02</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D28" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="11"/>
-      <c r="I28">
+      <c r="F28" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J28">
         <v>40</v>
       </c>
-      <c r="L28">
-        <f>I28</f>
+      <c r="M28">
+        <f>J28</f>
         <v>40</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D29" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="13"/>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <f t="shared" ref="L29:L39" si="6">I29</f>
-        <v>0</v>
-      </c>
-      <c r="O29" t="str">
-        <f>O28</f>
+      <c r="F29" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ref="M29:M39" si="6">J29</f>
+        <v>0</v>
+      </c>
+      <c r="P29" t="str">
+        <f>P28</f>
         <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D30" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="13"/>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="L30">
+      <c r="F30" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O30" t="str">
-        <f t="shared" ref="O30:O33" si="7">O29</f>
+      <c r="P30" t="str">
+        <f t="shared" ref="P30:P33" si="7">P29</f>
         <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>67</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="L31">
+      <c r="F31" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O31" t="str">
+      <c r="P31" t="str">
         <f t="shared" si="7"/>
         <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E32" s="13">
         <v>2030</v>
       </c>
-      <c r="I32" s="13">
+      <c r="F32" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J32" s="13">
         <v>0.98</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <f t="shared" si="6"/>
         <v>0.98</v>
       </c>
-      <c r="O32" t="str">
+      <c r="P32" t="str">
         <f t="shared" si="7"/>
         <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
-    <row r="33" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D33" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E33" s="13"/>
-      <c r="I33" s="13">
+      <c r="F33" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J33" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <f t="shared" si="6"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O33" t="str">
+      <c r="P33" t="str">
         <f t="shared" si="7"/>
         <v>TB_SUPCO2_DKISL2_DKW_01</v>
       </c>
     </row>
-    <row r="34" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D34" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E34" s="11"/>
-      <c r="I34">
+      <c r="F34" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J34">
         <v>40</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D35" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E35" s="13"/>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="L35">
+      <c r="F35" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="M35">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" t="str">
-        <f>O34</f>
+      <c r="P35" t="str">
+        <f>P34</f>
         <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
-    <row r="36" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D36" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E36" s="13"/>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="L36">
+      <c r="F36" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O36" t="str">
-        <f t="shared" ref="O36:O39" si="8">O35</f>
+      <c r="P36" t="str">
+        <f t="shared" ref="P36:P39" si="8">P35</f>
         <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
-    <row r="37" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>67</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="L37">
+      <c r="F37" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="M37">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O37" t="str">
+      <c r="P37" t="str">
         <f t="shared" si="8"/>
         <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
-    <row r="38" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D38" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="13">
         <v>2030</v>
       </c>
-      <c r="I38" s="13">
+      <c r="F38" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J38" s="13">
         <v>0.98</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <f t="shared" si="6"/>
         <v>0.98</v>
       </c>
-      <c r="O38" t="str">
+      <c r="P38" t="str">
         <f t="shared" si="8"/>
         <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
-    <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="13"/>
-      <c r="I39" s="13">
+      <c r="F39" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J39" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <f t="shared" si="6"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O39" t="str">
+      <c r="P39" t="str">
         <f t="shared" si="8"/>
         <v>TB_SUPCO2_DKISL2_DKW_02</v>
       </c>
     </row>
-    <row r="40" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D40" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="I40">
+      <c r="F40" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J40">
         <v>40</v>
       </c>
-      <c r="M40">
-        <f>I40</f>
+      <c r="N40">
+        <f>J40</f>
         <v>40</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D41" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E41" s="13"/>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <f t="shared" ref="M41:M51" si="9">I41</f>
-        <v>0</v>
-      </c>
-      <c r="O41" t="str">
-        <f>O40</f>
+      <c r="F41" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <f t="shared" ref="N41:N51" si="9">J41</f>
+        <v>0</v>
+      </c>
+      <c r="P41" t="str">
+        <f>P40</f>
         <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
-    <row r="42" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="13"/>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="M42">
+      <c r="F42" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="N42">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O42" t="str">
-        <f t="shared" ref="O42:O45" si="10">O41</f>
+      <c r="P42" t="str">
+        <f t="shared" ref="P42:P45" si="10">P41</f>
         <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
-    <row r="43" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>67</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="M43">
+      <c r="F43" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="N43">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O43" t="str">
+      <c r="P43" t="str">
         <f t="shared" si="10"/>
         <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
-    <row r="44" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D44" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E44" s="13">
         <v>2030</v>
       </c>
-      <c r="I44" s="13">
+      <c r="F44" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J44" s="13">
         <v>0.98</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <f t="shared" si="9"/>
         <v>0.98</v>
       </c>
-      <c r="O44" t="str">
+      <c r="P44" t="str">
         <f t="shared" si="10"/>
         <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
-    <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D45" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E45" s="13"/>
-      <c r="I45" s="13">
+      <c r="F45" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J45" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <f t="shared" si="9"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O45" t="str">
+      <c r="P45" t="str">
         <f t="shared" si="10"/>
         <v>TB_SUPCO2_DKISL3_DKW_01</v>
       </c>
     </row>
-    <row r="46" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D46" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="I46">
+      <c r="F46" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J46">
         <v>40</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D47" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E47" s="13"/>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="M47">
+      <c r="F47" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="N47">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O47" t="str">
-        <f>O46</f>
+      <c r="P47" t="str">
+        <f>P46</f>
         <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
-    <row r="48" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D48" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E48" s="13"/>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="M48">
+      <c r="F48" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="N48">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O48" t="str">
-        <f t="shared" ref="O48:O51" si="11">O47</f>
+      <c r="P48" t="str">
+        <f t="shared" ref="P48:P51" si="11">P47</f>
         <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>67</v>
       </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-      <c r="M49">
+      <c r="F49" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O49" t="str">
+      <c r="P49" t="str">
         <f t="shared" si="11"/>
         <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D50" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E50" s="13">
         <v>2030</v>
       </c>
-      <c r="I50" s="13">
+      <c r="F50" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J50" s="13">
         <v>0.98</v>
       </c>
-      <c r="M50">
+      <c r="N50">
         <f t="shared" si="9"/>
         <v>0.98</v>
       </c>
-      <c r="O50" t="str">
+      <c r="P50" t="str">
         <f t="shared" si="11"/>
         <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>
     </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D51" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="13"/>
-      <c r="I51" s="13">
+      <c r="F51" s="13">
+        <v>2030</v>
+      </c>
+      <c r="J51" s="13">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M51">
+      <c r="N51">
         <f t="shared" si="9"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O51" t="str">
+      <c r="P51" t="str">
         <f t="shared" si="11"/>
         <v>TB_SUPCO2_DKISL3_DKW_02</v>
       </c>

</xml_diff>

<commit_message>
Update ScenTrade_SUP_TRADE.xlsx by including price for Co2 ship transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_SUP_TRADE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223523C6-17EB-4DB5-AD24-E5A4621D776A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AFD3F1-0CA3-430A-839C-43F17DA92B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7164" yWindow="2004" windowWidth="30960" windowHeight="12204" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23412" windowHeight="15888" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+      <selection activeCell="J9" sqref="J9:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3440,7 +3440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6708D45-E573-4DB0-9E7B-7DC3BD947BD4}">
   <dimension ref="C2:AB44"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -4530,7 +4530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAD4FCC-23F0-4F3B-9CD2-8D3544B74DA5}">
   <dimension ref="C2:AA44"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -5627,7 +5627,7 @@
   <dimension ref="B2:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5718,12 +5718,12 @@
       <c r="F4" s="13">
         <v>2030</v>
       </c>
-      <c r="I4">
-        <v>40</v>
+      <c r="I4" s="11">
+        <v>50</v>
       </c>
       <c r="K4">
         <f>I4</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="P4" t="s">
         <v>68</v>
@@ -5737,12 +5737,12 @@
       <c r="F5" s="13">
         <v>2030</v>
       </c>
-      <c r="I5">
-        <v>0</v>
+      <c r="I5" s="13">
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K15" si="0">I5</f>
-        <v>0</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="P5" t="str">
         <f>P4</f>
@@ -5757,19 +5757,19 @@
       <c r="F6" s="13">
         <v>2030</v>
       </c>
-      <c r="I6">
-        <v>0</v>
+      <c r="I6" s="13">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ref="P6:P9" si="1">P5</f>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>67</v>
       </c>
@@ -5809,6 +5809,7 @@
         <f t="shared" si="1"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
+      <c r="U8" s="11"/>
     </row>
     <row r="9" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="13" t="s">
@@ -5829,6 +5830,7 @@
         <f t="shared" si="1"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
+      <c r="U9" s="13"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D10" s="11" t="s">
@@ -5839,15 +5841,16 @@
         <v>2030</v>
       </c>
       <c r="I10">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="P10" t="s">
         <v>69</v>
       </c>
+      <c r="U10" s="13"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D11" s="17" t="s">
@@ -5858,16 +5861,17 @@
         <v>2030</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="P11" t="str">
         <f>P10</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
+      <c r="U11" s="13"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D12" s="17" t="s">
@@ -5878,16 +5882,17 @@
         <v>2030</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" ref="P12:P15" si="2">P11</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
+      <c r="U12" s="14"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
@@ -5958,12 +5963,12 @@
       <c r="F16" s="13">
         <v>2030</v>
       </c>
-      <c r="J16">
-        <v>40</v>
+      <c r="J16" s="11">
+        <v>50</v>
       </c>
       <c r="L16">
         <f>J16</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="P16" t="s">
         <v>70</v>
@@ -5977,12 +5982,12 @@
       <c r="F17" s="13">
         <v>2030</v>
       </c>
-      <c r="J17">
-        <v>0</v>
+      <c r="J17" s="13">
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17:L27" si="3">J17</f>
-        <v>0</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="P17" t="str">
         <f>P16</f>
@@ -5997,12 +6002,12 @@
       <c r="F18" s="13">
         <v>2030</v>
       </c>
-      <c r="J18">
-        <v>0</v>
+      <c r="J18" s="13">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="L18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" ref="P18:P21" si="4">P17</f>
@@ -6079,11 +6084,11 @@
         <v>2030</v>
       </c>
       <c r="J22">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="L22">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="P22" t="s">
         <v>71</v>
@@ -6098,11 +6103,11 @@
         <v>2030</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="L23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="P23" t="str">
         <f>P22</f>
@@ -6118,11 +6123,11 @@
         <v>2030</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="L24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="P24" t="str">
         <f t="shared" ref="P24:P27" si="5">P23</f>
@@ -6198,12 +6203,12 @@
       <c r="F28" s="13">
         <v>2030</v>
       </c>
-      <c r="J28">
-        <v>40</v>
+      <c r="J28" s="11">
+        <v>50</v>
       </c>
       <c r="M28">
         <f>J28</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="P28" t="s">
         <v>72</v>
@@ -6217,12 +6222,12 @@
       <c r="F29" s="13">
         <v>2030</v>
       </c>
-      <c r="J29">
-        <v>0</v>
+      <c r="J29" s="13">
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="M29">
         <f t="shared" ref="M29:M39" si="6">J29</f>
-        <v>0</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="P29" t="str">
         <f>P28</f>
@@ -6237,12 +6242,12 @@
       <c r="F30" s="13">
         <v>2030</v>
       </c>
-      <c r="J30">
-        <v>0</v>
+      <c r="J30" s="13">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="M30">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="P30" t="str">
         <f t="shared" ref="P30:P33" si="7">P29</f>
@@ -6319,11 +6324,11 @@
         <v>2030</v>
       </c>
       <c r="J34">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="M34">
         <f t="shared" si="6"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="P34" t="s">
         <v>73</v>
@@ -6338,11 +6343,11 @@
         <v>2030</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="M35">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="P35" t="str">
         <f>P34</f>
@@ -6358,11 +6363,11 @@
         <v>2030</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="M36">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="P36" t="str">
         <f t="shared" ref="P36:P39" si="8">P35</f>
@@ -6438,12 +6443,12 @@
       <c r="F40" s="13">
         <v>2030</v>
       </c>
-      <c r="J40">
-        <v>40</v>
+      <c r="J40" s="11">
+        <v>50</v>
       </c>
       <c r="N40">
         <f>J40</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="P40" t="s">
         <v>74</v>
@@ -6457,12 +6462,12 @@
       <c r="F41" s="13">
         <v>2030</v>
       </c>
-      <c r="J41">
-        <v>0</v>
+      <c r="J41" s="13">
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="N41">
         <f t="shared" ref="N41:N51" si="9">J41</f>
-        <v>0</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="P41" t="str">
         <f>P40</f>
@@ -6477,12 +6482,12 @@
       <c r="F42" s="13">
         <v>2030</v>
       </c>
-      <c r="J42">
-        <v>0</v>
+      <c r="J42" s="13">
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="N42">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="P42" t="str">
         <f t="shared" ref="P42:P45" si="10">P41</f>
@@ -6559,11 +6564,11 @@
         <v>2030</v>
       </c>
       <c r="J46">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="N46">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="P46" t="s">
         <v>75</v>
@@ -6578,11 +6583,11 @@
         <v>2030</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="N47">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3.1329000000000001E-3</v>
       </c>
       <c r="P47" t="str">
         <f>P46</f>
@@ -6598,11 +6603,11 @@
         <v>2030</v>
       </c>
       <c r="J48">
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="N48">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.5659999999999999E-5</v>
       </c>
       <c r="P48" t="str">
         <f t="shared" ref="P48:P51" si="11">P47</f>

</xml_diff>